<commit_message>
login check, navigation check
</commit_message>
<xml_diff>
--- a/Styling/Responsive-Batch-1.xlsx
+++ b/Styling/Responsive-Batch-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\c-sharp-lab\ht2Journals\Styling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\epam-lab\c-sharp-lab\LLW_Framework\Styling\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -2256,7 +2253,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="31">
     <font>
       <sz val="11"/>
@@ -2776,9 +2773,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -13846,7 +13843,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75"/>
@@ -17063,21 +17060,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100664AEDDFEF44F9489F2399B746585A47" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="afc3b7e8c19a314cf5d880dfc6153292">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -17191,10 +17173,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E67CBCD6-85BF-4B50-8B6A-D46F74F86D1C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB611E9F-3B65-4361-B34B-EEE08367D984}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17215,17 +17220,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB611E9F-3B65-4361-B34B-EEE08367D984}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E67CBCD6-85BF-4B50-8B6A-D46F74F86D1C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>